<commit_message>
add lesson for two year
</commit_message>
<xml_diff>
--- a/public/uploads/data.xlsx
+++ b/public/uploads/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
   <si>
     <t>نام استاد</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>گسسته</t>
+  </si>
+  <si>
+    <t>96,97</t>
   </si>
   <si>
     <t>طراحی الگوریتم</t>
@@ -755,8 +758,8 @@
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="3">
-        <v>96.0</v>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="3">
         <v>10.0</v>
@@ -779,7 +782,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3">
         <v>96.0</v>
@@ -805,7 +808,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3">
         <v>97.0</v>
@@ -831,7 +834,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3">
         <v>96.0</v>
@@ -857,7 +860,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3">
         <v>96.0</v>
@@ -883,7 +886,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3">
         <v>98.0</v>
@@ -909,7 +912,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3">
         <v>97.0</v>
@@ -935,7 +938,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3">
         <v>98.0</v>
@@ -960,26 +963,26 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11">
-      <c r="B11" s="4"/>
+      <c r="B11" s="5"/>
     </row>
     <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13">
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14">
-      <c r="B14" s="4"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15">
-      <c r="B15" s="4"/>
+      <c r="B15" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="5"/>
+      <c r="A22" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1044,7 +1047,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
@@ -1052,7 +1055,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -1060,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
@@ -1068,7 +1071,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -1076,7 +1079,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
@@ -1084,7 +1087,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -1092,7 +1095,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1115,10 +1118,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1147,10 +1150,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1170,19 +1173,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2">
@@ -1190,16 +1193,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
@@ -1207,10 +1210,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
@@ -1218,15 +1221,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
@@ -1236,44 +1239,45 @@
     </row>
     <row r="14">
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C16" s="5"/>
     </row>
     <row r="17">
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>